<commit_message>
feat(Review): Positionierung Quellen, Abbildungen Achstentitel
</commit_message>
<xml_diff>
--- a/benchmarks/BenchmarksDiagrams.xlsx
+++ b/benchmarks/BenchmarksDiagrams.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ansgar\Documents\Development\Repositories\BunVsNodeJs\benchmarks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA4802C-AA4E-4F72-8036-7EFE8E0FCB1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77C6B9F5-D778-463D-8D57-D581301207F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{8F74B001-824D-4FE1-AEF6-C7F7EAAFBFDD}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8F74B001-824D-4FE1-AEF6-C7F7EAAFBFDD}"/>
   </bookViews>
   <sheets>
     <sheet name="HTTP-Server" sheetId="1" r:id="rId1"/>
@@ -52,9 +52,6 @@
     <t>Desktop-PC</t>
   </si>
   <si>
-    <t>Node.js 21.0.0</t>
-  </si>
-  <si>
     <t>Durchschnittliche Anfragen pro Sekunde (HTTP-Server)</t>
   </si>
   <si>
@@ -86,6 +83,9 @@
   </si>
   <si>
     <t>Ausführungszeit für die Berechnung der Fibonacci-Folge</t>
+  </si>
+  <si>
+    <t>Node.js Current</t>
   </si>
 </sst>
 </file>
@@ -166,7 +166,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -174,16 +174,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -419,7 +418,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Node.js 21.0.0</c:v>
+                  <c:v>Node.js Current</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -937,7 +936,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Node.js 21.0.0</c:v>
+                  <c:v>Node.js Current</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2270,7 +2269,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="de-DE"/>
-              <a:t>Durchschnittliche Latenz pro Sekunde auf dem Desktop-PC (File-Server)</a:t>
+              <a:t>Durchschnittliche Latenz auf dem Desktop-PC (File-Server)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2464,7 +2463,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Node.js Latest</c:v>
+                  <c:v>Node.js Current</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2612,6 +2611,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Durchschnittl. Latenz in ms</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2765,7 +2819,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="de-DE"/>
-              <a:t>Durchschnittliche Latenz pro Sekunde auf dem Macbook Pro (File-Server)</a:t>
+              <a:t>Durchschnittliche Latenz auf dem Macbook Pro (File-Server)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2959,7 +3013,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Node.js Latest</c:v>
+                  <c:v>Node.js Current</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3107,6 +3161,68 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Durchschnittl. Latenz in ms</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3428,7 +3544,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Node.js 21.0.0</c:v>
+                  <c:v>Node.js Current</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3563,6 +3679,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>CPU-Auslastung</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="de-DE" baseline="0"/>
+                  <a:t> in Prozent</a:t>
+                </a:r>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3884,7 +4060,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Node.js 21.0.0</c:v>
+                  <c:v>Node.js Current</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4403,7 +4579,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Node.js 21.0.0</c:v>
+                  <c:v>Node.js Current</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4538,6 +4714,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Ausführungszeit in Sekunden</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -10158,8 +10389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1066BB53-1D7C-4723-A7CA-755E56B72447}">
   <dimension ref="A2:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10168,11 +10399,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
+      <c r="A2" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
     </row>
     <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -10187,10 +10418,10 @@
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="5">
         <v>75685.819999999992</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>103215.08199999999</v>
       </c>
     </row>
@@ -10198,30 +10429,30 @@
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>45787.130000000005</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>30296.281999999999</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="6">
+        <v>15</v>
+      </c>
+      <c r="B6" s="5">
         <v>45881.502</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>32285.811999999998</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
+      <c r="A18" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
@@ -10235,10 +10466,10 @@
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="5">
         <v>6.6079999999999997</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="5">
         <v>4.8419999999999996</v>
       </c>
     </row>
@@ -10246,21 +10477,21 @@
       <c r="A21" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="5">
         <v>10.832000000000001</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C21" s="5">
         <v>16.502000000000002</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="6">
+        <v>15</v>
+      </c>
+      <c r="B22" s="5">
         <v>10.891999999999999</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C22" s="5">
         <v>15.489999999999998</v>
       </c>
     </row>
@@ -10278,8 +10509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{588F7207-FE6E-4A87-821C-C22620513FF6}">
   <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10293,19 +10524,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
     </row>
     <row r="2" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
@@ -10316,7 +10547,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="4" t="s">
@@ -10326,32 +10557,32 @@
         <v>1</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>50</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="7">
         <v>24761.913999999997</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="7">
         <v>11931.52</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="7">
         <v>14434.576000000001</v>
       </c>
       <c r="F3" s="3">
         <v>50</v>
       </c>
-      <c r="G3" s="10">
+      <c r="G3" s="8">
         <v>25299.227999999996</v>
       </c>
-      <c r="H3" s="10">
+      <c r="H3" s="8">
         <v>20767.222000000002</v>
       </c>
-      <c r="I3" s="10">
+      <c r="I3" s="8">
         <v>21636.044000000002</v>
       </c>
     </row>
@@ -10359,25 +10590,25 @@
       <c r="A4" s="3">
         <v>250</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="7">
         <v>24638.171999999999</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="7">
         <v>9373.3640000000014</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="7">
         <v>12041.237999999999</v>
       </c>
       <c r="F4" s="3">
         <v>250</v>
       </c>
-      <c r="G4" s="10">
+      <c r="G4" s="8">
         <v>25440.045999999998</v>
       </c>
-      <c r="H4" s="10">
+      <c r="H4" s="8">
         <v>16020.584000000003</v>
       </c>
-      <c r="I4" s="10">
+      <c r="I4" s="8">
         <v>17235.150000000001</v>
       </c>
     </row>
@@ -10385,25 +10616,25 @@
       <c r="A5" s="3">
         <v>100</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="7">
         <v>24155.311999999998</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="7">
         <v>8398.0025000000005</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="7">
         <v>10383.16</v>
       </c>
       <c r="F5" s="3">
         <v>100</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5" s="8">
         <v>23848.726000000002</v>
       </c>
-      <c r="H5" s="10">
+      <c r="H5" s="8">
         <v>14510.203999999998</v>
       </c>
-      <c r="I5" s="10">
+      <c r="I5" s="8">
         <v>14723.984</v>
       </c>
     </row>
@@ -10411,44 +10642,44 @@
       <c r="A6" s="3">
         <v>1000</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="7">
         <v>23786.799999999999</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="7">
         <v>7947.1539999999995</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="7">
         <v>8589.4560000000019</v>
       </c>
       <c r="F6" s="3">
         <v>1000</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G6" s="8">
         <v>24786.460000000003</v>
       </c>
-      <c r="H6" s="10">
+      <c r="H6" s="8">
         <v>14355.366</v>
       </c>
-      <c r="I6" s="10">
+      <c r="I6" s="8">
         <v>14684.222</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="4" t="s">
         <v>0</v>
@@ -10456,8 +10687,8 @@
       <c r="C26" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D26" s="4" t="s">
-        <v>7</v>
+      <c r="D26" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="3"/>
@@ -10467,33 +10698,33 @@
       <c r="H26" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="I26" s="4" t="s">
-        <v>7</v>
+      <c r="I26" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>50</v>
       </c>
-      <c r="B27" s="11">
+      <c r="B27" s="9">
         <v>2.0159999999999996</v>
       </c>
-      <c r="C27" s="11">
+      <c r="C27" s="9">
         <v>4.1680000000000001</v>
       </c>
-      <c r="D27" s="11">
+      <c r="D27" s="9">
         <v>3.4619999999999997</v>
       </c>
       <c r="F27" s="3">
         <v>50</v>
       </c>
-      <c r="G27" s="11">
+      <c r="G27" s="9">
         <v>1.9760000000000002</v>
       </c>
-      <c r="H27" s="11">
+      <c r="H27" s="9">
         <v>2.4119999999999999</v>
       </c>
-      <c r="I27" s="11">
+      <c r="I27" s="9">
         <v>2.3079999999999998</v>
       </c>
     </row>
@@ -10501,25 +10732,25 @@
       <c r="A28" s="3">
         <v>250</v>
       </c>
-      <c r="B28" s="11">
+      <c r="B28" s="9">
         <v>10.146000000000001</v>
       </c>
-      <c r="C28" s="11">
+      <c r="C28" s="9">
         <v>26.610000000000003</v>
       </c>
-      <c r="D28" s="11">
+      <c r="D28" s="9">
         <v>20.756</v>
       </c>
       <c r="F28" s="3">
         <v>250</v>
       </c>
-      <c r="G28" s="11">
+      <c r="G28" s="9">
         <v>9.8260000000000005</v>
       </c>
-      <c r="H28" s="11">
+      <c r="H28" s="9">
         <v>15.563999999999998</v>
       </c>
-      <c r="I28" s="11">
+      <c r="I28" s="9">
         <v>12.661999999999999</v>
       </c>
     </row>
@@ -10527,25 +10758,25 @@
       <c r="A29" s="3">
         <v>100</v>
       </c>
-      <c r="B29" s="11">
+      <c r="B29" s="9">
         <v>20.694000000000003</v>
       </c>
-      <c r="C29" s="11">
+      <c r="C29" s="9">
         <v>58.814999999999991</v>
       </c>
-      <c r="D29" s="11">
+      <c r="D29" s="9">
         <v>47.752499999999998</v>
       </c>
       <c r="F29" s="3">
         <v>100</v>
       </c>
-      <c r="G29" s="11">
+      <c r="G29" s="9">
         <v>20.957999999999998</v>
       </c>
-      <c r="H29" s="11">
+      <c r="H29" s="9">
         <v>34.456000000000003</v>
       </c>
-      <c r="I29" s="11">
+      <c r="I29" s="9">
         <v>33.953999999999994</v>
       </c>
     </row>
@@ -10553,45 +10784,45 @@
       <c r="A30" s="3">
         <v>1000</v>
       </c>
-      <c r="B30" s="11">
+      <c r="B30" s="9">
         <v>42.094000000000001</v>
       </c>
-      <c r="C30" s="11">
+      <c r="C30" s="9">
         <v>126.15799999999999</v>
       </c>
-      <c r="D30" s="11">
+      <c r="D30" s="9">
         <v>115.76799999999999</v>
       </c>
       <c r="F30" s="3">
         <v>1000</v>
       </c>
-      <c r="G30" s="11">
+      <c r="G30" s="9">
         <v>40.332000000000001</v>
       </c>
-      <c r="H30" s="11">
+      <c r="H30" s="9">
         <v>69.722000000000008</v>
       </c>
-      <c r="I30" s="11">
+      <c r="I30" s="9">
         <v>67.998000000000005</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L41" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
+      <c r="A47" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B47" s="11"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="4"/>
+      <c r="F47" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B47" s="5"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="7"/>
-      <c r="F47" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G47" s="5"/>
-      <c r="H47" s="5"/>
+      <c r="G47" s="11"/>
+      <c r="H47" s="11"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B48" s="3" t="s">
@@ -10612,20 +10843,20 @@
       <c r="A49" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B49" s="12">
+      <c r="B49" s="10">
         <v>55.543999999999997</v>
       </c>
-      <c r="C49" s="12">
+      <c r="C49" s="10">
         <v>82.661600000000007</v>
       </c>
-      <c r="D49" s="8"/>
+      <c r="D49" s="6"/>
       <c r="F49" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G49" s="10">
+      <c r="G49" s="8">
         <v>90.6</v>
       </c>
-      <c r="H49" s="10">
+      <c r="H49" s="8">
         <v>96.2</v>
       </c>
     </row>
@@ -10633,41 +10864,41 @@
       <c r="A50" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B50" s="12">
+      <c r="B50" s="10">
         <v>295.36</v>
       </c>
-      <c r="C50" s="12">
+      <c r="C50" s="10">
         <v>151.8672</v>
       </c>
-      <c r="D50" s="8"/>
+      <c r="D50" s="6"/>
       <c r="F50" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G50" s="10">
+      <c r="G50" s="8">
         <v>195</v>
       </c>
-      <c r="H50" s="10">
+      <c r="H50" s="8">
         <v>167.4</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B51" s="12">
+        <v>15</v>
+      </c>
+      <c r="B51" s="10">
         <v>330.48</v>
       </c>
-      <c r="C51" s="12">
+      <c r="C51" s="10">
         <v>211.56559999999999</v>
       </c>
-      <c r="D51" s="8"/>
+      <c r="D51" s="6"/>
       <c r="F51" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G51" s="10">
+        <v>15</v>
+      </c>
+      <c r="G51" s="8">
         <v>204.6</v>
       </c>
-      <c r="H51" s="10">
+      <c r="H51" s="8">
         <v>279.60000000000002</v>
       </c>
     </row>
@@ -10689,8 +10920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1E32A47-C85F-4D2E-BFDE-D8820CE9A189}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10701,11 +10932,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
+      <c r="A1" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -10720,10 +10951,10 @@
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="5">
         <v>3.2439999999999998</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="5">
         <v>4.4719999999999995</v>
       </c>
     </row>
@@ -10731,21 +10962,21 @@
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="5">
         <v>6.5060000000000002</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>7.346000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="6">
+        <v>15</v>
+      </c>
+      <c r="B5" s="5">
         <v>6.3220000000000001</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>7.1800000000000015</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: fehlende Diagramme hinzugefügt und verlinkt
</commit_message>
<xml_diff>
--- a/benchmarks/BenchmarksDiagrams.xlsx
+++ b/benchmarks/BenchmarksDiagrams.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ansgar\Documents\Development\Repositories\BunVsNodeJs\benchmarks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77C6B9F5-D778-463D-8D57-D581301207F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3975A3EE-7456-4CBB-9A52-13A2FB7C5B24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8F74B001-824D-4FE1-AEF6-C7F7EAAFBFDD}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{8F74B001-824D-4FE1-AEF6-C7F7EAAFBFDD}"/>
   </bookViews>
   <sheets>
     <sheet name="HTTP-Server" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="18">
   <si>
     <t>Bun</t>
   </si>
@@ -86,6 +86,12 @@
   </si>
   <si>
     <t>Node.js Current</t>
+  </si>
+  <si>
+    <t>CPU-Auslastung bei der Berechnung der Fibonacci-Folge</t>
+  </si>
+  <si>
+    <t>RAM-Nutzung bei der Berechnung der Fibonacci-Folge</t>
   </si>
 </sst>
 </file>
@@ -691,6 +697,1035 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>CPU-Auslastung bei der Berechnung der Fibonacci-Folge</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="de-DE" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:endParaRPr lang="de-DE" b="0"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Fibonacci!$F$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Bun</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Fibonacci!$G$1:$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>MacBook Pro</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Desktop-PC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Fibonacci!$G$3:$H$3</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7E8B-4AFB-A03F-685C0BF669B7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Fibonacci!$F$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Node.js LTS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Fibonacci!$G$1:$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>MacBook Pro</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Desktop-PC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Fibonacci!$G$4:$H$4</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>99.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7E8B-4AFB-A03F-685C0BF669B7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Fibonacci!$F$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Node.js Current</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Fibonacci!$G$1:$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>MacBook Pro</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Desktop-PC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Fibonacci!$G$5:$H$5</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>99.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-7E8B-4AFB-A03F-685C0BF669B7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1587288927"/>
+        <c:axId val="1593339295"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1587288927"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1593339295"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1593339295"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>CPu-Auslastung in Prozent</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1587288927"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>RAM-Nutzung bei der Berechnung der Fibonacci-Folge</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="de-DE" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:endParaRPr lang="de-DE" b="0"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Fibonacci!$A$27</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Bun</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Fibonacci!$B$25:$C$26</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>MacBook Pro</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Desktop-PC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Fibonacci!$B$27:$C$27</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>25.926400000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44.847000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FF6D-47D6-BBD0-831965FBA51D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Fibonacci!$A$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Node.js LTS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Fibonacci!$B$25:$C$26</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>MacBook Pro</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Desktop-PC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Fibonacci!$B$28:$C$28</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>41.977600000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>46.156799999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FF6D-47D6-BBD0-831965FBA51D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Fibonacci!$A$29</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Node.js Current</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Fibonacci!$B$25:$C$26</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>MacBook Pro</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Desktop-PC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Fibonacci!$B$29:$C$29</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>36.735999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43.827199999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-FF6D-47D6-BBD0-831965FBA51D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1694938207"/>
+        <c:axId val="1693180719"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1694938207"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1693180719"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1693180719"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>RAM-Nutzung in Megabyte</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1694938207"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -4924,6 +5959,80 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors10.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent4"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors11.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent4"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
   <a:schemeClr val="accent6"/>
@@ -5221,6 +6330,1012 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style10.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style11.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -10087,6 +12202,78 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Diagramm 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{108B9DB0-01DF-39E7-1D53-A05B9112CB3B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>23812</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>423862</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Diagramm 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BF263A1-1365-77FB-EB68-EB0C12394207}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -10389,7 +12576,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1066BB53-1D7C-4723-A7CA-755E56B72447}">
   <dimension ref="A2:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
@@ -10918,10 +13105,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1E32A47-C85F-4D2E-BFDE-D8820CE9A189}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10929,16 +13116,25 @@
     <col min="1" max="1" width="31.7109375" customWidth="1"/>
     <col min="2" max="2" width="40.5703125" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>14</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
+      <c r="F1" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
     </row>
-    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="3" t="s">
         <v>2</v>
@@ -10946,8 +13142,15 @@
       <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -10957,8 +13160,17 @@
       <c r="C3" s="5">
         <v>4.4719999999999995</v>
       </c>
+      <c r="F3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="5">
+        <v>100</v>
+      </c>
+      <c r="H3" s="5">
+        <v>100</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -10968,8 +13180,17 @@
       <c r="C4" s="5">
         <v>7.346000000000001</v>
       </c>
+      <c r="F4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="5">
+        <v>99</v>
+      </c>
+      <c r="H4" s="5">
+        <v>99.2</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
@@ -10979,10 +13200,70 @@
       <c r="C5" s="5">
         <v>7.1800000000000015</v>
       </c>
+      <c r="F5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="5">
+        <v>99</v>
+      </c>
+      <c r="H5" s="5">
+        <v>99.6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+    </row>
+    <row r="26" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27">
+        <v>25.926400000000001</v>
+      </c>
+      <c r="C27" s="5">
+        <v>44.847000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28">
+        <v>41.977600000000002</v>
+      </c>
+      <c r="C28" s="5">
+        <v>46.156799999999997</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29">
+        <v>36.735999999999997</v>
+      </c>
+      <c r="C29" s="5">
+        <v>43.827199999999998</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="A1:C1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="A25:C25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
refactor: Feedback Markus unklare Kommentare
</commit_message>
<xml_diff>
--- a/benchmarks/BenchmarksDiagrams.xlsx
+++ b/benchmarks/BenchmarksDiagrams.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ansgar\Documents\Development\Repositories\BunVsNodeJs\benchmarks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3975A3EE-7456-4CBB-9A52-13A2FB7C5B24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D70F14-A56B-4C3C-9536-7CED4DBCA474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{8F74B001-824D-4FE1-AEF6-C7F7EAAFBFDD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8F74B001-824D-4FE1-AEF6-C7F7EAAFBFDD}"/>
   </bookViews>
   <sheets>
     <sheet name="HTTP-Server" sheetId="1" r:id="rId1"/>
@@ -172,7 +172,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -189,6 +189,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -5013,7 +5014,7 @@
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>55.543999999999997</c:v>
+                  <c:v>67.827200000000005</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>82.661600000000007</c:v>
@@ -12576,7 +12577,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1066BB53-1D7C-4723-A7CA-755E56B72447}">
   <dimension ref="A2:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
@@ -12696,8 +12697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{588F7207-FE6E-4A87-821C-C22620513FF6}">
   <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13030,8 +13031,8 @@
       <c r="A49" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B49" s="10">
-        <v>55.543999999999997</v>
+      <c r="B49" s="12">
+        <v>67.827200000000005</v>
       </c>
       <c r="C49" s="10">
         <v>82.661600000000007</v>
@@ -13107,7 +13108,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1E32A47-C85F-4D2E-BFDE-D8820CE9A189}">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>

</xml_diff>